<commit_message>
Testing dataset is little bit off cannot process it
</commit_message>
<xml_diff>
--- a/2D Data/Different Model Analysis Report.xlsx
+++ b/2D Data/Different Model Analysis Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Nit Durgapur\College 4th Sem\JU Internship\Fins Heat Prediction\2D Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0478907D-1824-427F-9ED3-9159B80E131A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129CBB8-C913-4288-9708-AA3FE26F1A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{DED646A6-1EB9-4F3B-930A-09C6ED4DF818}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{DED646A6-1EB9-4F3B-930A-09C6ED4DF818}"/>
   </bookViews>
   <sheets>
     <sheet name="Try 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Try 3" sheetId="3" r:id="rId3"/>
     <sheet name="Try 4" sheetId="4" r:id="rId4"/>
     <sheet name="Try 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Try 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Try 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Try 9" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="76">
   <si>
     <t>2D Model Analysis</t>
   </si>
@@ -230,6 +233,42 @@
   </si>
   <si>
     <t>9 min 32.5 sec</t>
+  </si>
+  <si>
+    <t>Without using regulizers and learning rate = 0.0001, optimizers patience = 5 and y is scaled using StandardScaler(). Also we are using mse as loss function</t>
+  </si>
+  <si>
+    <t>Loss (mse)</t>
+  </si>
+  <si>
+    <t>49 -&gt; 56</t>
+  </si>
+  <si>
+    <t>9 min 8.40 sec</t>
+  </si>
+  <si>
+    <t>Without using regulizers and learning rate = 0.001, optimizers patience = 5 and y is scaled using RobustScaler(). Also we are using hubber loss as loss function</t>
+  </si>
+  <si>
+    <t>Input Layer = Dense(512, )</t>
+  </si>
+  <si>
+    <t>Dense(256, swish)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss </t>
+  </si>
+  <si>
+    <t>Huber loss</t>
+  </si>
+  <si>
+    <t>115 -&gt; 129</t>
+  </si>
+  <si>
+    <t>18 min 44 sec</t>
+  </si>
+  <si>
+    <t>Dense (64)</t>
   </si>
 </sst>
 </file>
@@ -408,12 +447,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -426,13 +459,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,6 +472,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -782,30 +821,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E4" s="3" t="s">
@@ -859,8 +898,8 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -885,13 +924,13 @@
       <c r="I9" s="5">
         <v>6.4755000000000003</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="6">
         <v>5.2584</v>
       </c>
       <c r="K9" s="5">
         <v>33</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -914,13 +953,13 @@
       <c r="I10" s="5">
         <v>6.3768000000000002</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="6">
         <v>5.2131999999999996</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -939,13 +978,13 @@
       <c r="I11" s="5">
         <v>6.1062000000000003</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="6">
         <v>5.0547000000000004</v>
       </c>
       <c r="K11" s="5">
         <v>34</v>
       </c>
-      <c r="L11" s="13"/>
+      <c r="L11" s="17"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -959,8 +998,8 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -989,7 +1028,7 @@
       <c r="K13" s="5">
         <v>70</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="L13" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1013,7 +1052,7 @@
       <c r="K14" s="5">
         <v>70</v>
       </c>
-      <c r="L14" s="12"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E15" s="5"/>
@@ -1035,7 +1074,7 @@
       <c r="K15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="12"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E16" s="5"/>
@@ -1055,7 +1094,7 @@
       <c r="K16" s="5">
         <v>73</v>
       </c>
-      <c r="L16" s="13"/>
+      <c r="L16" s="17"/>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E17" s="2"/>
@@ -1087,7 +1126,7 @@
         <v>20.435300000000002</v>
       </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="11"/>
+      <c r="L18" s="15"/>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E19" s="5"/>
@@ -1105,7 +1144,7 @@
         <v>9.3183000000000007</v>
       </c>
       <c r="K19" s="5"/>
-      <c r="L19" s="12"/>
+      <c r="L19" s="16"/>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E20" s="5"/>
@@ -1123,7 +1162,7 @@
         <v>8.3505000000000003</v>
       </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="13"/>
+      <c r="L20" s="17"/>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
@@ -1157,7 +1196,7 @@
       <c r="K22" s="5">
         <v>83</v>
       </c>
-      <c r="L22" s="11" t="s">
+      <c r="L22" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1181,7 +1220,7 @@
       <c r="K23" s="5">
         <v>81</v>
       </c>
-      <c r="L23" s="12"/>
+      <c r="L23" s="16"/>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E24" s="5"/>
@@ -1201,7 +1240,7 @@
       <c r="K24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L24" s="12"/>
+      <c r="L24" s="16"/>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E25" s="5"/>
@@ -1221,7 +1260,7 @@
       <c r="K25" s="5">
         <v>82</v>
       </c>
-      <c r="L25" s="13"/>
+      <c r="L25" s="17"/>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E26" s="2"/>
@@ -1253,7 +1292,7 @@
         <v>34.2089</v>
       </c>
       <c r="K27" s="5"/>
-      <c r="L27" s="11"/>
+      <c r="L27" s="15"/>
     </row>
     <row r="28" spans="5:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E28" s="5"/>
@@ -1273,7 +1312,7 @@
         <v>15.9057</v>
       </c>
       <c r="K28" s="5"/>
-      <c r="L28" s="12"/>
+      <c r="L28" s="16"/>
     </row>
     <row r="29" spans="5:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E29" s="5"/>
@@ -1293,7 +1332,7 @@
         <v>12.808</v>
       </c>
       <c r="K29" s="5"/>
-      <c r="L29" s="13"/>
+      <c r="L29" s="17"/>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E30" s="2"/>
@@ -1327,7 +1366,7 @@
       <c r="K31" s="5">
         <v>131</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="L31" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1351,7 +1390,7 @@
       <c r="K32" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L32" s="12"/>
+      <c r="L32" s="16"/>
     </row>
     <row r="33" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
@@ -1371,23 +1410,24 @@
       <c r="K33" s="5">
         <v>93</v>
       </c>
-      <c r="L33" s="13"/>
+      <c r="L33" s="17"/>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="17"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="14"/>
     </row>
     <row r="35" spans="5:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:J2"/>
     <mergeCell ref="E34:L34"/>
     <mergeCell ref="L9:L11"/>
     <mergeCell ref="L13:L16"/>
@@ -1395,7 +1435,6 @@
     <mergeCell ref="L18:L20"/>
     <mergeCell ref="L27:L29"/>
     <mergeCell ref="L31:L33"/>
-    <mergeCell ref="A1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1452,13 +1491,13 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1482,10 +1521,10 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -1507,12 +1546,12 @@
       <c r="G9" s="5">
         <v>55</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1533,10 +1572,10 @@
       <c r="G10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1555,82 +1594,82 @@
       <c r="G11" s="5">
         <v>53</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="5" t="s">
         <v>53</v>
       </c>
@@ -1639,19 +1678,19 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1735,13 +1774,13 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1765,10 +1804,10 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -1790,12 +1829,12 @@
       <c r="G9" s="5">
         <v>50</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1816,10 +1855,10 @@
       <c r="G10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1838,70 +1877,70 @@
       <c r="G11" s="5">
         <v>53</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5" t="s">
         <v>53</v>
       </c>
@@ -1910,19 +1949,19 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1940,7 +1979,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,13 +2045,13 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
@@ -2036,8 +2075,8 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -2061,12 +2100,12 @@
       <c r="G9" s="5">
         <v>62</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="15" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2087,10 +2126,10 @@
       <c r="G10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="5" t="s">
         <v>58</v>
       </c>
@@ -2109,70 +2148,70 @@
       <c r="G11" s="5">
         <v>59</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5" t="s">
         <v>53</v>
       </c>
@@ -2181,19 +2220,19 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2210,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D9C69D-0E21-4580-903F-FCC6540D49FC}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2277,13 +2316,13 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
@@ -2307,8 +2346,8 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -2332,12 +2371,12 @@
       <c r="G9" s="5">
         <v>71</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2358,10 +2397,10 @@
       <c r="G10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="5" t="s">
         <v>58</v>
       </c>
@@ -2380,70 +2419,70 @@
       <c r="G11" s="5">
         <v>69</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5" t="s">
         <v>53</v>
       </c>
@@ -2452,19 +2491,809 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="H9:H17"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:H18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735F7089-1D64-4AF1-9CE8-89C1047B155E}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61.21875" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.32390000000000002</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="F9" s="5">
+        <v>50</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.22309999999999999</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.21229999999999999</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.1273</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="F11" s="5">
+        <v>49</v>
+      </c>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="G9:G17"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:G18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F15A2-EB6A-41E4-8815-F0985D7D8327}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3.3224</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4.3823999999999996</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3.6831</v>
+      </c>
+      <c r="G9" s="5">
+        <v>129</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2.6070000000000002</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3.4188999999999998</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2.9661</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8399000000000001</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.3765999999999998</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2.2128000000000001</v>
+      </c>
+      <c r="G11" s="5">
+        <v>131</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="H9:H17"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:H18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCBB9F9-67EF-4443-A471-CDB5B90EAA7E}">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3.3224</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4.3823999999999996</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3.6831</v>
+      </c>
+      <c r="G9" s="5">
+        <v>129</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2.6070000000000002</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3.4188999999999998</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2.9661</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8399000000000001</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.3765999999999998</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2.2128000000000001</v>
+      </c>
+      <c r="G11" s="5">
+        <v>131</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Model is 90% complete
</commit_message>
<xml_diff>
--- a/2D Data/Different Model Analysis Report.xlsx
+++ b/2D Data/Different Model Analysis Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Nit Durgapur\College 4th Sem\JU Internship\Fins Heat Prediction\2D Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129CBB8-C913-4288-9708-AA3FE26F1A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCEB895-4872-4FDB-B35E-42CD84D161FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{DED646A6-1EB9-4F3B-930A-09C6ED4DF818}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{DED646A6-1EB9-4F3B-930A-09C6ED4DF818}"/>
   </bookViews>
   <sheets>
     <sheet name="Try 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Try 6" sheetId="6" r:id="rId6"/>
     <sheet name="Try 7" sheetId="7" r:id="rId7"/>
     <sheet name="Try 9" sheetId="8" r:id="rId8"/>
+    <sheet name="Try 10" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="83">
   <si>
     <t>2D Model Analysis</t>
   </si>
@@ -268,7 +269,28 @@
     <t>18 min 44 sec</t>
   </si>
   <si>
-    <t>Dense (64)</t>
+    <t>Input Layer = Dense(128, )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huber loss, no regularizers, learning rate = 0.01, x and y scaled by MinMaxScaler()  </t>
+  </si>
+  <si>
+    <t>57 -&gt; 44</t>
+  </si>
+  <si>
+    <t>4 min 36.0 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huber loss, no regularizers, learning rate = 0.001, x and y scaled by MinMaxScaler()  </t>
+  </si>
+  <si>
+    <t>Dense(16, swish)</t>
+  </si>
+  <si>
+    <t>40 -&gt; 58</t>
+  </si>
+  <si>
+    <t>8 min 26.5 sec</t>
   </si>
 </sst>
 </file>
@@ -2768,7 +2790,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2895,7 +2917,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>68</v>
       </c>
@@ -3038,15 +3060,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCBB9F9-67EF-4443-A471-CDB5B90EAA7E}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="54.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -3058,7 +3084,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -3068,7 +3094,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -3082,7 +3108,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3092,7 +3118,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3102,12 +3128,12 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
@@ -3125,11 +3151,8 @@
       <c r="H7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3139,7 +3162,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -3150,24 +3173,24 @@
         <v>12</v>
       </c>
       <c r="D9" s="5">
-        <v>3.3224</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="E9" s="5">
-        <v>4.3823999999999996</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="F9" s="5">
-        <v>3.6831</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="G9" s="5">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>21</v>
@@ -3176,42 +3199,42 @@
         <v>31</v>
       </c>
       <c r="D10" s="5">
-        <v>2.6070000000000002</v>
+        <v>2.8E-3</v>
       </c>
       <c r="E10" s="5">
-        <v>3.4188999999999998</v>
+        <v>2.8E-3</v>
       </c>
       <c r="F10" s="5">
-        <v>2.9661</v>
+        <v>3.7199999999999997E-2</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="5">
-        <v>1.8399000000000001</v>
+        <v>2.3E-3</v>
       </c>
       <c r="E11" s="5">
-        <v>2.3765999999999998</v>
+        <v>2.3E-3</v>
       </c>
       <c r="F11" s="5">
-        <v>2.2128000000000001</v>
+        <v>3.5099999999999999E-2</v>
       </c>
       <c r="G11" s="5">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>30</v>
@@ -3223,7 +3246,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>21</v>
@@ -3235,10 +3258,10 @@
       <c r="G13" s="5"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3247,7 +3270,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>21</v>
@@ -3259,10 +3282,10 @@
       <c r="G15" s="5"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3271,36 +3294,331 @@
       <c r="G16" s="5"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
       <c r="B17" s="5" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H2"/>
-    <mergeCell ref="H9:H17"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="H9:H18"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="A19:H19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D442498-2B1F-421B-9AF3-D4948F00BF73}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5.96E-2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>50</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4.1500000000000002E-2</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.3E-3</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3.27E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>59</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="H9:H18"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="A19:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>